<commit_message>
afe bom part added
</commit_message>
<xml_diff>
--- a/BMS_doc/AFE_PCB_BOM.xlsx
+++ b/BMS_doc/AFE_PCB_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GF_BMS\BMS_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7BC2E2-A61D-4BFA-BD79-2C0F62EF5891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3D0C1B-DA07-4230-A997-52F17139EF2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12210" windowHeight="4980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="200">
   <si>
     <t>SCH-MCU_AFE           Revision: 01</t>
   </si>
@@ -608,6 +608,18 @@
   </si>
   <si>
     <t xml:space="preserve">10 POSITION SINGLE ROW STRIEGHT FEMALE SOCKET TH 2.0MM </t>
+  </si>
+  <si>
+    <t>C74,C75,C76,C77,C78,C79,C90</t>
+  </si>
+  <si>
+    <t>1000PF</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V 10% X7R 0402</t>
+  </si>
+  <si>
+    <t>04025C102KAT2A</t>
   </si>
 </sst>
 </file>
@@ -661,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -687,6 +699,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1001,11 +1017,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20:XFD20"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1386,339 +1402,339 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" t="s">
+    <row r="14" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="G15" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="I17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>192</v>
+        <v>71</v>
       </c>
       <c r="E18" t="s">
-        <v>193</v>
+        <v>72</v>
       </c>
       <c r="G18" t="s">
-        <v>186</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>187</v>
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
       </c>
       <c r="I18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="D19" t="s">
-        <v>194</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>195</v>
+        <v>192</v>
+      </c>
+      <c r="E19" t="s">
+        <v>193</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" t="s">
-        <v>77</v>
+        <v>186</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>187</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" t="s">
-        <v>81</v>
+        <v>194</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="G20" t="s">
         <v>74</v>
       </c>
       <c r="H20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="H21" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="H22" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I22" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23">
-        <v>39</v>
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G23" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="H23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D24">
-        <v>127</v>
+        <v>39</v>
       </c>
       <c r="E24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="I24" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="D25">
+        <v>127</v>
       </c>
       <c r="E25" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
         <v>101</v>
       </c>
       <c r="H25" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I25" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1">
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G26" t="s">
         <v>101</v>
       </c>
       <c r="H26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="I26" t="s">
         <v>93</v>
@@ -1726,25 +1742,25 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E27" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
         <v>101</v>
       </c>
       <c r="H27" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="I27" t="s">
         <v>93</v>
@@ -1752,25 +1768,25 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E28" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G28" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="H28" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I28" t="s">
         <v>93</v>
@@ -1778,282 +1794,282 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29">
-        <v>10</v>
+        <v>116</v>
+      </c>
+      <c r="D29" t="s">
+        <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="H29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="I29" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>31</v>
-      </c>
-      <c r="B30" s="3">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G30" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I30" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D31">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H31" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I31" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G32" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H32" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="I32" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>125</v>
+      </c>
+      <c r="G33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" t="s">
+        <v>126</v>
+      </c>
+      <c r="I33" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>35</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>131</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>132</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>133</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G34" t="s">
         <v>134</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>135</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>36</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D35" s="5">
         <v>22.2</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E35" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G35" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>37</v>
-      </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" t="s">
-        <v>140</v>
-      </c>
-      <c r="E35" t="s">
-        <v>141</v>
-      </c>
-      <c r="G35" t="s">
-        <v>142</v>
-      </c>
-      <c r="H35" t="s">
-        <v>140</v>
-      </c>
-      <c r="I35" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36" s="1">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="H36" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="I36" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E37" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="G37" t="s">
-        <v>152</v>
+        <v>69</v>
       </c>
       <c r="H37" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I37" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E38" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G38" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="H38" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="I38" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E39" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G39" t="s">
         <v>142</v>
       </c>
       <c r="H39" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I39" t="s">
         <v>157</v>
@@ -2061,143 +2077,165 @@
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E40" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G40" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="H40" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="I40" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>43</v>
-      </c>
-      <c r="B41" s="3">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E41" t="s">
-        <v>168</v>
-      </c>
-      <c r="F41" t="s">
-        <v>169</v>
+        <v>163</v>
+      </c>
+      <c r="G41" t="s">
+        <v>164</v>
+      </c>
+      <c r="H41" t="s">
+        <v>162</v>
+      </c>
+      <c r="I41" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" s="3">
-        <v>2</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>171</v>
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42" t="s">
+        <v>168</v>
+      </c>
+      <c r="F42" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B43" s="3">
         <v>2</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="C43" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>47</v>
+      </c>
+      <c r="B44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G44" s="5" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>49</v>
-      </c>
-      <c r="B44" s="3">
-        <v>3</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="I44" s="5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
+        <v>49</v>
+      </c>
+      <c r="B45" s="3">
+        <v>3</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>50</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B46" s="3">
         <v>4</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="G46" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="H46" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="I45" s="7" t="s">
+      <c r="I46" s="7" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
@@ -5982,6 +6020,10 @@
     <row r="992" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A992" s="1"/>
       <c r="B992" s="1"/>
+    </row>
+    <row r="993" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A993" s="1"/>
+      <c r="B993" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
bom afe part added
</commit_message>
<xml_diff>
--- a/BMS_doc/AFE_PCB_BOM.xlsx
+++ b/BMS_doc/AFE_PCB_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GF_BMS\BMS_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C95533-C1B1-4710-B010-060D36CC545A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ACD5DE-DB58-46FB-94CB-B18992A26FEE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12210" windowHeight="4980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="199">
   <si>
     <t>SCH-MCU_AFE           Revision: 01</t>
   </si>
@@ -608,6 +608,15 @@
   </si>
   <si>
     <t>C87</t>
+  </si>
+  <si>
+    <t>CRM2512-FX-1000ELF</t>
+  </si>
+  <si>
+    <t>BOURNS - SMD Current Sense Resistor, 100 ohm, CRM Series, 2512 [6432 Metric], 2 W, ± 1%, Thick Film</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-charge resistor </t>
   </si>
 </sst>
 </file>
@@ -661,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -683,14 +692,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,8 +1018,8 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1017,7 +1027,7 @@
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="71.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="30.42578125" customWidth="1"/>
@@ -1027,9 +1037,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1055,11 +1065,11 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1390,29 +1400,29 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+    <row r="14" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
         <v>12</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>7</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2184,6 +2194,15 @@
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
+      <c r="C47" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>

</xml_diff>